<commit_message>
Update spider results 2025-12-03 02:48:30
</commit_message>
<xml_diff>
--- a/cx.xlsx
+++ b/cx.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,6 +438,40 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>关于准予撤销上海市徐汇区柳州路邮政所的公告</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2025-12-02</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202512/be58981880de42c7822366e7faabd2cb.shtml</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>关于准予撤销上海市松江区达丰邮政所的公告</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202510/e5a44a5099d1476fa0e479b321267ac3.shtml</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update spider results 2025-12-03 03:05:48
</commit_message>
<xml_diff>
--- a/cx.xlsx
+++ b/cx.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,40 +438,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>关于准予撤销上海市徐汇区柳州路邮政所的公告</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>2025-12-02</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202512/be58981880de42c7822366e7faabd2cb.shtml</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>关于准予撤销上海市松江区达丰邮政所的公告</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2025-10-31</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202510/e5a44a5099d1476fa0e479b321267ac3.shtml</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update spider results 2025-12-09 02:51:30
</commit_message>
<xml_diff>
--- a/cx.xlsx
+++ b/cx.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,6 +438,57 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>关于准予撤销上海市嘉定区朱家桥邮政支局的公告</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2025-12-05</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202512/b487344d328e4d2fa163d4fe9a0fe502.shtml</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>关于准予撤销上海市徐汇区柳州路邮政所的公告</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2025-12-02</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202512/be58981880de42c7822366e7faabd2cb.shtml</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>关于准予撤销上海市松江区达丰邮政所的公告</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202510/e5a44a5099d1476fa0e479b321267ac3.shtml</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update spider results 2025-12-11 03:01:45
</commit_message>
<xml_diff>
--- a/cx.xlsx
+++ b/cx.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,57 +438,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>关于准予撤销上海市嘉定区朱家桥邮政支局的公告</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>2025-12-05</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202512/b487344d328e4d2fa163d4fe9a0fe502.shtml</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>关于准予撤销上海市徐汇区柳州路邮政所的公告</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2025-12-02</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202512/be58981880de42c7822366e7faabd2cb.shtml</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>关于准予撤销上海市松江区达丰邮政所的公告</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>2025-10-31</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202510/e5a44a5099d1476fa0e479b321267ac3.shtml</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update spider results 2025-12-17 02:54:08
</commit_message>
<xml_diff>
--- a/cx.xlsx
+++ b/cx.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,6 +438,57 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>关于准予撤销上海市嘉定区朱家桥邮政支局的公告</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2025-12-05</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202512/b487344d328e4d2fa163d4fe9a0fe502.shtml</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>关于准予撤销上海市徐汇区柳州路邮政所的公告</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2025-12-02</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202512/be58981880de42c7822366e7faabd2cb.shtml</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>关于准予撤销上海市松江区达丰邮政所的公告</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202510/e5a44a5099d1476fa0e479b321267ac3.shtml</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update spider results 2025-12-18 02:57:31
</commit_message>
<xml_diff>
--- a/cx.xlsx
+++ b/cx.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,57 +438,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>关于准予撤销上海市嘉定区朱家桥邮政支局的公告</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>2025-12-05</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202512/b487344d328e4d2fa163d4fe9a0fe502.shtml</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>关于准予撤销上海市徐汇区柳州路邮政所的公告</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2025-12-02</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202512/be58981880de42c7822366e7faabd2cb.shtml</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>关于准予撤销上海市松江区达丰邮政所的公告</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>2025-10-31</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202510/e5a44a5099d1476fa0e479b321267ac3.shtml</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update spider results 2025-12-24 02:56:05
</commit_message>
<xml_diff>
--- a/cx.xlsx
+++ b/cx.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,6 +438,57 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>关于准予撤销上海市嘉定区朱家桥邮政支局的公告</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2025-12-05</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202512/b487344d328e4d2fa163d4fe9a0fe502.shtml</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>关于准予撤销上海市徐汇区柳州路邮政所的公告</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2025-12-02</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202512/be58981880de42c7822366e7faabd2cb.shtml</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>关于准予撤销上海市松江区达丰邮政所的公告</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202510/e5a44a5099d1476fa0e479b321267ac3.shtml</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update spider results 2025-12-25 03:04:13
</commit_message>
<xml_diff>
--- a/cx.xlsx
+++ b/cx.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,57 +438,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>关于准予撤销上海市嘉定区朱家桥邮政支局的公告</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>2025-12-05</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202512/b487344d328e4d2fa163d4fe9a0fe502.shtml</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>关于准予撤销上海市徐汇区柳州路邮政所的公告</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2025-12-02</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202512/be58981880de42c7822366e7faabd2cb.shtml</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>关于准予撤销上海市松江区达丰邮政所的公告</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>2025-10-31</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202510/e5a44a5099d1476fa0e479b321267ac3.shtml</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update spider results 2025-12-28 03:11:06
</commit_message>
<xml_diff>
--- a/cx.xlsx
+++ b/cx.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,6 +438,57 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>关于准予撤销上海市嘉定区朱家桥邮政支局的公告</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2025-12-05</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202512/b487344d328e4d2fa163d4fe9a0fe502.shtml</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>关于准予撤销上海市徐汇区柳州路邮政所的公告</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2025-12-02</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202512/be58981880de42c7822366e7faabd2cb.shtml</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>关于准予撤销上海市松江区达丰邮政所的公告</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202510/e5a44a5099d1476fa0e479b321267ac3.shtml</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update spider results 2025-12-30 03:05:03
</commit_message>
<xml_diff>
--- a/cx.xlsx
+++ b/cx.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,57 +438,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>关于准予撤销上海市嘉定区朱家桥邮政支局的公告</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>2025-12-05</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202512/b487344d328e4d2fa163d4fe9a0fe502.shtml</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>关于准予撤销上海市徐汇区柳州路邮政所的公告</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2025-12-02</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202512/be58981880de42c7822366e7faabd2cb.shtml</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>关于准予撤销上海市松江区达丰邮政所的公告</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>2025-10-31</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202510/e5a44a5099d1476fa0e479b321267ac3.shtml</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update spider results 2026-01-01 03:11:26
</commit_message>
<xml_diff>
--- a/cx.xlsx
+++ b/cx.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,6 +438,57 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>关于准予撤销上海市嘉定区朱家桥邮政支局的公告</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2025-12-05</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202512/b487344d328e4d2fa163d4fe9a0fe502.shtml</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>关于准予撤销上海市徐汇区柳州路邮政所的公告</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2025-12-02</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202512/be58981880de42c7822366e7faabd2cb.shtml</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>关于准予撤销上海市松江区达丰邮政所的公告</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202510/e5a44a5099d1476fa0e479b321267ac3.shtml</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update spider results 2026-01-03 02:57:46
</commit_message>
<xml_diff>
--- a/cx.xlsx
+++ b/cx.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,57 +438,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>关于准予撤销上海市嘉定区朱家桥邮政支局的公告</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>2025-12-05</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202512/b487344d328e4d2fa163d4fe9a0fe502.shtml</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>关于准予撤销上海市徐汇区柳州路邮政所的公告</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2025-12-02</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202512/be58981880de42c7822366e7faabd2cb.shtml</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>关于准予撤销上海市松江区达丰邮政所的公告</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>2025-10-31</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202510/e5a44a5099d1476fa0e479b321267ac3.shtml</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update spider results 2026-01-23 03:03:54
</commit_message>
<xml_diff>
--- a/cx.xlsx
+++ b/cx.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,6 +438,57 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>关于准予撤销上海市嘉定区朱家桥邮政支局的公告</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2025-12-05</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202512/b487344d328e4d2fa163d4fe9a0fe502.shtml</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>关于准予撤销上海市徐汇区柳州路邮政所的公告</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2025-12-02</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202512/be58981880de42c7822366e7faabd2cb.shtml</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>关于准予撤销上海市松江区达丰邮政所的公告</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202510/e5a44a5099d1476fa0e479b321267ac3.shtml</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update spider results 2026-01-24 03:02:27
</commit_message>
<xml_diff>
--- a/cx.xlsx
+++ b/cx.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,57 +438,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>关于准予撤销上海市嘉定区朱家桥邮政支局的公告</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>2025-12-05</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202512/b487344d328e4d2fa163d4fe9a0fe502.shtml</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>关于准予撤销上海市徐汇区柳州路邮政所的公告</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2025-12-02</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202512/be58981880de42c7822366e7faabd2cb.shtml</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>关于准予撤销上海市松江区达丰邮政所的公告</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>2025-10-31</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202510/e5a44a5099d1476fa0e479b321267ac3.shtml</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update spider results 2026-01-26 03:20:09
</commit_message>
<xml_diff>
--- a/cx.xlsx
+++ b/cx.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,6 +438,57 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>关于准予撤销上海市嘉定区朱家桥邮政支局的公告</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2025-12-05</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202512/b487344d328e4d2fa163d4fe9a0fe502.shtml</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>关于准予撤销上海市徐汇区柳州路邮政所的公告</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2025-12-02</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202512/be58981880de42c7822366e7faabd2cb.shtml</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>关于准予撤销上海市松江区达丰邮政所的公告</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202510/e5a44a5099d1476fa0e479b321267ac3.shtml</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update spider results 2026-01-27 03:13:10
</commit_message>
<xml_diff>
--- a/cx.xlsx
+++ b/cx.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,57 +438,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>关于准予撤销上海市嘉定区朱家桥邮政支局的公告</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>2025-12-05</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202512/b487344d328e4d2fa163d4fe9a0fe502.shtml</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>关于准予撤销上海市徐汇区柳州路邮政所的公告</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2025-12-02</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202512/be58981880de42c7822366e7faabd2cb.shtml</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>关于准予撤销上海市松江区达丰邮政所的公告</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>2025-10-31</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202510/e5a44a5099d1476fa0e479b321267ac3.shtml</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update spider results 2026-01-28 03:06:45
</commit_message>
<xml_diff>
--- a/cx.xlsx
+++ b/cx.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,6 +438,57 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>关于准予撤销上海市嘉定区朱家桥邮政支局的公告</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2025-12-05</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202512/b487344d328e4d2fa163d4fe9a0fe502.shtml</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>关于准予撤销上海市徐汇区柳州路邮政所的公告</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2025-12-02</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202512/be58981880de42c7822366e7faabd2cb.shtml</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>关于准予撤销上海市松江区达丰邮政所的公告</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202510/e5a44a5099d1476fa0e479b321267ac3.shtml</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update spider results 2026-01-29 03:34:37
</commit_message>
<xml_diff>
--- a/cx.xlsx
+++ b/cx.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,57 +438,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>关于准予撤销上海市嘉定区朱家桥邮政支局的公告</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>2025-12-05</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202512/b487344d328e4d2fa163d4fe9a0fe502.shtml</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>关于准予撤销上海市徐汇区柳州路邮政所的公告</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2025-12-02</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202512/be58981880de42c7822366e7faabd2cb.shtml</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>关于准予撤销上海市松江区达丰邮政所的公告</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>2025-10-31</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202510/e5a44a5099d1476fa0e479b321267ac3.shtml</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update spider results 2026-02-06 03:35:16
</commit_message>
<xml_diff>
--- a/cx.xlsx
+++ b/cx.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,6 +438,40 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>关于准予撤销上海市嘉定区朱家桥邮政支局的公告</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2025-12-05</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202512/b487344d328e4d2fa163d4fe9a0fe502.shtml</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>关于准予撤销上海市徐汇区柳州路邮政所的公告</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2025-12-02</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202512/be58981880de42c7822366e7faabd2cb.shtml</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update spider results 2026-02-07 03:33:00
</commit_message>
<xml_diff>
--- a/cx.xlsx
+++ b/cx.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,40 +438,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>关于准予撤销上海市嘉定区朱家桥邮政支局的公告</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>2025-12-05</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202512/b487344d328e4d2fa163d4fe9a0fe502.shtml</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>关于准予撤销上海市徐汇区柳州路邮政所的公告</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2025-12-02</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202512/be58981880de42c7822366e7faabd2cb.shtml</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update spider results 2026-02-09 03:46:55
</commit_message>
<xml_diff>
--- a/cx.xlsx
+++ b/cx.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,6 +438,40 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>关于准予撤销上海市嘉定区朱家桥邮政支局的公告</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2025-12-05</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202512/b487344d328e4d2fa163d4fe9a0fe502.shtml</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>关于准予撤销上海市徐汇区柳州路邮政所的公告</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2025-12-02</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202512/be58981880de42c7822366e7faabd2cb.shtml</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update spider results 2026-02-10 03:57:46
</commit_message>
<xml_diff>
--- a/cx.xlsx
+++ b/cx.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,40 +438,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>关于准予撤销上海市嘉定区朱家桥邮政支局的公告</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>2025-12-05</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202512/b487344d328e4d2fa163d4fe9a0fe502.shtml</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>关于准予撤销上海市徐汇区柳州路邮政所的公告</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2025-12-02</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202512/be58981880de42c7822366e7faabd2cb.shtml</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update spider results 2026-02-13 03:45:11
</commit_message>
<xml_diff>
--- a/cx.xlsx
+++ b/cx.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,6 +438,40 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>关于准予撤销上海市嘉定区朱家桥邮政支局的公告</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2025-12-05</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202512/b487344d328e4d2fa163d4fe9a0fe502.shtml</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>关于准予撤销上海市徐汇区柳州路邮政所的公告</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2025-12-02</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202512/be58981880de42c7822366e7faabd2cb.shtml</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update spider results 2026-02-14 03:36:17
</commit_message>
<xml_diff>
--- a/cx.xlsx
+++ b/cx.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,40 +438,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>关于准予撤销上海市嘉定区朱家桥邮政支局的公告</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>2025-12-05</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202512/b487344d328e4d2fa163d4fe9a0fe502.shtml</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>关于准予撤销上海市徐汇区柳州路邮政所的公告</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2025-12-02</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202512/be58981880de42c7822366e7faabd2cb.shtml</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update spider results 2026-02-17 03:41:57
</commit_message>
<xml_diff>
--- a/cx.xlsx
+++ b/cx.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,6 +438,40 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>关于准予撤销上海市嘉定区朱家桥邮政支局的公告</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2025-12-05</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202512/b487344d328e4d2fa163d4fe9a0fe502.shtml</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>关于准予撤销上海市徐汇区柳州路邮政所的公告</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2025-12-02</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202512/be58981880de42c7822366e7faabd2cb.shtml</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update spider results 2026-02-18 03:46:31
</commit_message>
<xml_diff>
--- a/cx.xlsx
+++ b/cx.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,40 +438,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>关于准予撤销上海市嘉定区朱家桥邮政支局的公告</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>2025-12-05</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202512/b487344d328e4d2fa163d4fe9a0fe502.shtml</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>关于准予撤销上海市徐汇区柳州路邮政所的公告</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2025-12-02</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202512/be58981880de42c7822366e7faabd2cb.shtml</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update spider results 2026-02-19 03:43:44
</commit_message>
<xml_diff>
--- a/cx.xlsx
+++ b/cx.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,6 +438,40 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>关于准予撤销上海市嘉定区朱家桥邮政支局的公告</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2025-12-05</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202512/b487344d328e4d2fa163d4fe9a0fe502.shtml</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>关于准予撤销上海市徐汇区柳州路邮政所的公告</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2025-12-02</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202512/be58981880de42c7822366e7faabd2cb.shtml</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update spider results 2026-02-20 03:39:55
</commit_message>
<xml_diff>
--- a/cx.xlsx
+++ b/cx.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,40 +438,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>关于准予撤销上海市嘉定区朱家桥邮政支局的公告</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>2025-12-05</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202512/b487344d328e4d2fa163d4fe9a0fe502.shtml</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>关于准予撤销上海市徐汇区柳州路邮政所的公告</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2025-12-02</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202512/be58981880de42c7822366e7faabd2cb.shtml</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update spider results 2026-02-24 03:40:58
</commit_message>
<xml_diff>
--- a/cx.xlsx
+++ b/cx.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,6 +438,40 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>关于准予撤销上海市嘉定区朱家桥邮政支局的公告</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2025-12-05</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202512/b487344d328e4d2fa163d4fe9a0fe502.shtml</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>关于准予撤销上海市徐汇区柳州路邮政所的公告</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2025-12-02</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202512/be58981880de42c7822366e7faabd2cb.shtml</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update spider results 2026-02-25 03:44:38
</commit_message>
<xml_diff>
--- a/cx.xlsx
+++ b/cx.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,40 +438,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>关于准予撤销上海市嘉定区朱家桥邮政支局的公告</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>2025-12-05</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202512/b487344d328e4d2fa163d4fe9a0fe502.shtml</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>关于准予撤销上海市徐汇区柳州路邮政所的公告</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2025-12-02</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202512/be58981880de42c7822366e7faabd2cb.shtml</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update spider results 2026-02-27 03:33:46
</commit_message>
<xml_diff>
--- a/cx.xlsx
+++ b/cx.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,6 +438,40 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>关于准予撤销上海市嘉定区朱家桥邮政支局的公告</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2025-12-05</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202512/b487344d328e4d2fa163d4fe9a0fe502.shtml</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>关于准予撤销上海市徐汇区柳州路邮政所的公告</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2025-12-02</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202512/be58981880de42c7822366e7faabd2cb.shtml</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update spider results 2026-02-28 03:17:18
</commit_message>
<xml_diff>
--- a/cx.xlsx
+++ b/cx.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,40 +438,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>关于准予撤销上海市嘉定区朱家桥邮政支局的公告</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>2025-12-05</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202512/b487344d328e4d2fa163d4fe9a0fe502.shtml</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>关于准予撤销上海市徐汇区柳州路邮政所的公告</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2025-12-02</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>https://sh.spb.gov.cn/shsyzglj/c100057/c100058/202512/be58981880de42c7822366e7faabd2cb.shtml</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>